<commit_message>
Updated the test log with more pictures
</commit_message>
<xml_diff>
--- a/testing/eyeDetectionTestingLog.xlsx
+++ b/testing/eyeDetectionTestingLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="16275" windowHeight="7485"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="67">
   <si>
     <t>Web Location</t>
   </si>
@@ -179,12 +179,90 @@
   <si>
     <t xml:space="preserve">Nostril selected </t>
   </si>
+  <si>
+    <t>http://faceresearch.org/uploads/base/african_male.jpg</t>
+  </si>
+  <si>
+    <t>Brian Nguyen</t>
+  </si>
+  <si>
+    <t>http://www.co.bibb.ga.us/TaxAssessors/images/JGordonMask.jpg</t>
+  </si>
+  <si>
+    <t>Part of eyebrow and mustache elected</t>
+  </si>
+  <si>
+    <t>http://www.standardmedia.co.ke/images/friday/Angola250113.jpg</t>
+  </si>
+  <si>
+    <t>http://everyafricanwoman.files.wordpress.com/2012/08/575034_429235650450940_156056494_n.jpg</t>
+  </si>
+  <si>
+    <t>Eye detection window does not appear</t>
+  </si>
+  <si>
+    <t>http://maricopa360.com/wp-content/uploads/2009/03/raymon-tapia.jpg</t>
+  </si>
+  <si>
+    <t>http://us.123rf.com/400wm/400/400/barsik/barsik0707/barsik070700006/1200772-portrait-of-a-young-mexican-girl-laughing.jpg</t>
+  </si>
+  <si>
+    <t>Detects corner of mouth</t>
+  </si>
+  <si>
+    <t>http://www.goworldtravel.com/june05/j0227709.jpg</t>
+  </si>
+  <si>
+    <t>Only detects right eye</t>
+  </si>
+  <si>
+    <t>http://1.bp.blogspot.com/-L2PBaae9jOs/TdKFi09IaSI/AAAAAAAAAKE/1Y3ymlfNDeE/s1600/indian+male+4+whysoindian.jpg</t>
+  </si>
+  <si>
+    <t>http://faceresearch.org/uploads/base/eastasian_male.jpg</t>
+  </si>
+  <si>
+    <t>http://0.tqn.com/d/menshair/1/0/H/A/-/-/01.jpg</t>
+  </si>
+  <si>
+    <t>http://asianfilmfestla.org/2012/wp-content/uploads/2012/04/2012_lum_debbie_seeking_asian_female.jpg</t>
+  </si>
+  <si>
+    <t>http://www.beautyanalysis.com/images/PG-45B---RF---Asian-Female-.jpg</t>
+  </si>
+  <si>
+    <t>http://noahsdad.com/wp-content/2012/05/baby-down-syndrome-face-boy-smiling-9.jpg</t>
+  </si>
+  <si>
+    <t>Detects part of the forehead</t>
+  </si>
+  <si>
+    <t>http://anthro.palomar.edu/abnormal/images/Down_Syndrome_child.jpg</t>
+  </si>
+  <si>
+    <t>Doesn't detect eyes</t>
+  </si>
+  <si>
+    <t>http://www.pyroenergen.com/articles07/images/d-syndrome2.jpg</t>
+  </si>
+  <si>
+    <t>http://s3.amazonaws.com/rapgenius/lazy-eye-treatment.jpg</t>
+  </si>
+  <si>
+    <t>http://www.thehealthage.com/site/wp-content/uploads/2010/10/lazy-eye.jpg</t>
+  </si>
+  <si>
+    <t>http://t3.gstatic.com/images?q=tbn:ANd9GcSpfRlvwWWm3T6lSmwpq_a09LVgrB92POV8yjeVhp4awRINl--H</t>
+  </si>
+  <si>
+    <t>Only detect left eye</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,7 +323,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -269,6 +347,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -276,6 +355,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -354,6 +438,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -388,6 +473,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -563,14 +649,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
@@ -579,7 +665,7 @@
     <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="30">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -596,7 +682,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="210">
+    <row r="2" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -613,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="210">
+    <row r="3" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -630,7 +716,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135">
+    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -647,7 +733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="135">
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -664,7 +750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105">
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -681,7 +767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105">
+    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -698,7 +784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -715,7 +801,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -732,7 +818,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -749,7 +835,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="135">
+    <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -766,7 +852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="120">
+    <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -783,7 +869,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="90">
+    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -800,7 +886,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -817,7 +903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="195">
+    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -834,7 +920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="210">
+    <row r="16" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -851,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90">
+    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -868,7 +954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="120">
+    <row r="18" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -885,7 +971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75">
+    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -902,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="75">
+    <row r="20" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
@@ -917,6 +1003,312 @@
       </c>
       <c r="E20" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -939,32 +1331,50 @@
     <hyperlink ref="A15" r:id="rId16"/>
     <hyperlink ref="A17" r:id="rId17"/>
     <hyperlink ref="A20" r:id="rId18"/>
+    <hyperlink ref="A21" r:id="rId19"/>
+    <hyperlink ref="A22" r:id="rId20"/>
+    <hyperlink ref="A23" r:id="rId21"/>
+    <hyperlink ref="A24" r:id="rId22"/>
+    <hyperlink ref="A25" r:id="rId23"/>
+    <hyperlink ref="A26" r:id="rId24"/>
+    <hyperlink ref="A27" r:id="rId25"/>
+    <hyperlink ref="A28" r:id="rId26"/>
+    <hyperlink ref="A29" r:id="rId27"/>
+    <hyperlink ref="A30" r:id="rId28"/>
+    <hyperlink ref="A31" r:id="rId29"/>
+    <hyperlink ref="A32" r:id="rId30"/>
+    <hyperlink ref="A33" r:id="rId31"/>
+    <hyperlink ref="A34" r:id="rId32"/>
+    <hyperlink ref="A35" r:id="rId33"/>
+    <hyperlink ref="A36" r:id="rId34"/>
+    <hyperlink ref="A37" r:id="rId35"/>
+    <hyperlink ref="A38" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
-  <legacyDrawing r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
+  <legacyDrawing r:id="rId38"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
retested some photos to make sure error handling works
</commit_message>
<xml_diff>
--- a/testing/eyeDetectionTestingLog.xlsx
+++ b/testing/eyeDetectionTestingLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="150" windowWidth="16275" windowHeight="7485"/>
@@ -136,14 +136,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>Traceback (most recent call last):
-  File "C:\Users\Shannon\Documents\GitHub\DVS-Python\eyeDetection.py", line 99, in &lt;module&gt;
-    image = DetectRedEyes(img, faceCascade, eyeCascade)
-  File "C:\Users\Shannon\Documents\GitHub\DVS-Python\eyeDetection.py", line 71, in DetectRedEyes
-    cv.SetImageROI(image, (pt1[0],
-UnboundLocalError: local variable 'pt1' referenced before assignment</t>
-  </si>
-  <si>
     <t>Nostril and right ear falsely recognized</t>
   </si>
   <si>
@@ -256,13 +248,16 @@
   </si>
   <si>
     <t>Only detect left eye</t>
+  </si>
+  <si>
+    <t>SystemExit: No faces were found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,7 +433,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -473,7 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -649,14 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
@@ -665,7 +658,7 @@
     <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="30">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -682,7 +675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="210">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -699,7 +692,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="90">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -707,16 +700,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4">
-        <v>41389</v>
+        <v>41400</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="135">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -733,7 +726,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="135">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -741,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4">
         <v>41389</v>
@@ -750,7 +743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="105">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -758,7 +751,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="4">
         <v>41389</v>
@@ -767,16 +760,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="105">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="D7" s="4">
         <v>41389</v>
       </c>
@@ -784,7 +777,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -792,7 +785,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
         <v>41389</v>
@@ -801,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="75">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -818,7 +811,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -835,7 +828,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="135">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -843,7 +836,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="4">
         <v>41389</v>
@@ -852,7 +845,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="120">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -860,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4">
         <v>41389</v>
@@ -869,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="90">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -877,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="4">
         <v>41389</v>
@@ -886,7 +879,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="60">
       <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
@@ -894,7 +887,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4">
         <v>41389</v>
@@ -903,7 +896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="195">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
@@ -920,7 +913,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="120">
       <c r="A16" s="5" t="s">
         <v>21</v>
       </c>
@@ -928,16 +921,16 @@
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="D16" s="4">
-        <v>41389</v>
+        <v>41400</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="90">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -945,7 +938,7 @@
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="4">
         <v>41389</v>
@@ -954,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="120">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -962,7 +955,7 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="4">
         <v>41389</v>
@@ -971,7 +964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="75">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -988,15 +981,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45.75" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="D20" s="4">
         <v>41391</v>
@@ -1005,9 +998,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="39.75" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>26</v>
@@ -1019,296 +1012,296 @@
         <v>41397</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="39" customHeight="1">
+      <c r="A22" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="B23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
+      <c r="B24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="3" t="s">
+      <c r="D24" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="B25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+      <c r="B26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="3" t="s">
+      <c r="D27" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D27" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+      <c r="B28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+      <c r="B29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
+      <c r="B30" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="9" t="s">
+      <c r="B31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="B32" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D33" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="B34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="3" t="s">
+      <c r="D34" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="B35" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D35" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="B36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="9" t="s">
+      <c r="B37" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="4">
+        <v>41397</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="4">
-        <v>41397</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="s">
+      <c r="B38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="D38" s="4">
         <v>41397</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1357,24 +1350,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Random files I haven't commited
</commit_message>
<xml_diff>
--- a/testing/eyeDetectionTestingLog.xlsx
+++ b/testing/eyeDetectionTestingLog.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="76">
   <si>
     <t>Web Location</t>
   </si>
@@ -225,14 +225,69 @@
     <t>http://web.archive.org/web/20130225135511/http://noahsdad.com/wp-content/2012/05/baby-down-syndrome-face-boy-smiling-9.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Success Rate </t>
+    <t>Ideal/Workable Photo?</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>No - black and white</t>
+  </si>
+  <si>
+    <t>No - painting</t>
+  </si>
+  <si>
+    <t>No - not a full head</t>
+  </si>
+  <si>
+    <t>No - too close, looking sideways</t>
+  </si>
+  <si>
+    <t>No - face paint and hat</t>
+  </si>
+  <si>
+    <t>No - soft focus, tilted gaze</t>
+  </si>
+  <si>
+    <t>No - strange angle</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No - lots of jewelry</t>
+  </si>
+  <si>
+    <t>No - watermark on photo</t>
+  </si>
+  <si>
+    <t>No - squinting</t>
+  </si>
+  <si>
+    <t>No - doesn’t have full head</t>
+  </si>
+  <si>
+    <t>Maybe - looking a bit down</t>
+  </si>
+  <si>
+    <t>Success Rate - All</t>
+  </si>
+  <si>
+    <t>Success Rate - Ideal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+No - looking sideways, odd shadow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +330,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -301,7 +362,7 @@
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
@@ -329,6 +390,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -633,22 +695,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="30">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="30">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -664,8 +727,11 @@
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" customHeight="1">
+      <c r="F1" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>24</v>
       </c>
@@ -679,7 +745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="33.75" customHeight="1">
+    <row r="3" spans="1:7" ht="33.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -695,8 +761,12 @@
       <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="27" customHeight="1">
+      <c r="F3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="27" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -712,8 +782,11 @@
       <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="16.5" customHeight="1">
+      <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -727,7 +800,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="120">
+    <row r="6" spans="1:7" ht="150">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -743,8 +816,11 @@
       <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1">
+      <c r="F6" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="18" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -760,8 +836,11 @@
       <c r="E7" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="14.25" customHeight="1">
+      <c r="F7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -778,7 +857,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="14.25" customHeight="1">
+    <row r="9" spans="1:7" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -795,7 +874,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1">
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -812,8 +891,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="17.25" customHeight="1">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" ht="17.25" customHeight="1">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -828,8 +907,11 @@
       <c r="E11" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="17.25" customHeight="1">
+      <c r="F11" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="17.25" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -846,7 +928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="17.25" customHeight="1">
+    <row r="13" spans="1:7" ht="17.25" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -862,8 +944,11 @@
       <c r="E13" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="16.5" customHeight="1">
+      <c r="F13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -879,8 +964,11 @@
       <c r="E14" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1">
+      <c r="F14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="13.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -897,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.5" customHeight="1">
+    <row r="16" spans="1:7" ht="16.5" customHeight="1">
       <c r="A16" s="5" t="s">
         <v>20</v>
       </c>
@@ -913,8 +1001,11 @@
       <c r="E16" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F16" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -930,8 +1021,11 @@
       <c r="E17" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="31.5" customHeight="1">
+      <c r="F17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="31.5" customHeight="1">
       <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
@@ -947,8 +1041,11 @@
       <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="F18" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
@@ -965,7 +1062,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="17.25" customHeight="1">
+    <row r="20" spans="1:6" ht="17.25" customHeight="1">
       <c r="A20" s="5" t="s">
         <v>29</v>
       </c>
@@ -981,8 +1078,11 @@
       <c r="E20" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="18" customHeight="1">
+      <c r="F20" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="18" customHeight="1">
       <c r="A21" s="9" t="s">
         <v>30</v>
       </c>
@@ -999,7 +1099,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.5" customHeight="1">
+    <row r="22" spans="1:6" ht="16.5" customHeight="1">
       <c r="A22" s="9" t="s">
         <v>31</v>
       </c>
@@ -1016,7 +1116,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="A23" s="9" t="s">
         <v>32</v>
       </c>
@@ -1033,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:6">
       <c r="A24" s="9" t="s">
         <v>33</v>
       </c>
@@ -1049,8 +1149,11 @@
       <c r="E24" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="9" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6" ht="30">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -1083,8 +1186,11 @@
       <c r="E26" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="9" t="s">
         <v>36</v>
       </c>
@@ -1100,8 +1206,11 @@
       <c r="E27" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="9" t="s">
         <v>37</v>
       </c>
@@ -1118,7 +1227,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" s="9" t="s">
         <v>38</v>
       </c>
@@ -1135,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:6">
       <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
@@ -1152,7 +1261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:6">
       <c r="A31" s="9" t="s">
         <v>40</v>
       </c>
@@ -1169,7 +1278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:6">
       <c r="A32" s="9" t="s">
         <v>41</v>
       </c>
@@ -1186,7 +1295,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:6">
       <c r="A33" s="9" t="s">
         <v>56</v>
       </c>
@@ -1203,7 +1312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:6">
       <c r="A34" s="9" t="s">
         <v>42</v>
       </c>
@@ -1219,8 +1328,11 @@
       <c r="E34" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="9" t="s">
         <v>44</v>
       </c>
@@ -1237,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:6" ht="30">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -1253,8 +1365,11 @@
       <c r="E36" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="9" t="s">
         <v>46</v>
       </c>
@@ -1271,7 +1386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:6" ht="30">
       <c r="A38" s="9" t="s">
         <v>47</v>
       </c>
@@ -1287,20 +1402,25 @@
       <c r="E38" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F38" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="30">
       <c r="A40" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B40" s="10">
-        <f>(37-17)/37</f>
-        <v>0.54054054054054057</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B40" s="10"/>
       <c r="D40" s="4">
         <v>41419</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1341,10 +1461,11 @@
     <hyperlink ref="A37" r:id="rId34"/>
     <hyperlink ref="A38" r:id="rId35"/>
     <hyperlink ref="A33" r:id="rId36" display="http://web.archive.org/web/20130225135511/http:/noahsdad.com/wp-content/2012/05/baby-down-syndrome-face-boy-smiling-9.jpg"/>
+    <hyperlink ref="A11" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId37"/>
-  <legacyDrawing r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId38"/>
+  <legacyDrawing r:id="rId39"/>
 </worksheet>
 </file>
 

</xml_diff>